<commit_message>
Success Note for QC Reject
</commit_message>
<xml_diff>
--- a/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
+++ b/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/AICA008_Incoming List (Supplier)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D45CEABF-4239-4CBC-A092-39BB24B0637B}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7B2CE3-81D5-4E3A-B4B2-4C985BE20399}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2715" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DS APAC" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Item code</t>
   </si>
@@ -188,6 +188,60 @@
   </si>
   <si>
     <t>FG-01-4137-1-1200-1</t>
+  </si>
+  <si>
+    <t>RW-09-8415-2-05-0</t>
+  </si>
+  <si>
+    <t>OIL Yellow 3G-05KG/CAN</t>
+  </si>
+  <si>
+    <t>RW-09-8502-2-50-0</t>
+  </si>
+  <si>
+    <t>CALCIUM OXIDE-50KG/BAG</t>
+  </si>
+  <si>
+    <t>RW-09-8504-2-25-0</t>
+  </si>
+  <si>
+    <t>RW-09-8507-2-25-0</t>
+  </si>
+  <si>
+    <t>RW-09-8508-2-20-0</t>
+  </si>
+  <si>
+    <t>RW-09-8509-2-30-0</t>
+  </si>
+  <si>
+    <t>RW-09-8701-2-25-0</t>
+  </si>
+  <si>
+    <t>RW-09-8704-2-10-0</t>
+  </si>
+  <si>
+    <t>Note for line 11</t>
+  </si>
+  <si>
+    <t>Note for line 12</t>
+  </si>
+  <si>
+    <t>Note for line 13</t>
+  </si>
+  <si>
+    <t>Note for line 14</t>
+  </si>
+  <si>
+    <t>Note for line 15</t>
+  </si>
+  <si>
+    <t>Note for line 16</t>
+  </si>
+  <si>
+    <t>Note for line 17</t>
+  </si>
+  <si>
+    <t>Note for line 18</t>
   </si>
 </sst>
 </file>
@@ -764,10 +818,10 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1183,6 +1237,142 @@
         <v>38</v>
       </c>
     </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1200</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1200</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1200</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1200</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="4">
+        <v>250</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="4">
+        <v>250</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="4">
+        <v>250</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1200</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:F22">
     <sortCondition ref="B12:B22"/>
@@ -1194,7 +1384,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{84CCA402-EF47-4CC8-A3D1-DDDBFF7E0782}"/>
+      <autoFilter ref="A2:F2" xr:uid="{79C6C58C-F30E-4A61-853B-E1A60DB1FA9B}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Retrofited Swal on incoming list. Qc not completed
</commit_message>
<xml_diff>
--- a/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
+++ b/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="222" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7B2CE3-81D5-4E3A-B4B2-4C985BE20399}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DS APAC" sheetId="1" r:id="rId1"/>
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1384,7 +1384,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{79C6C58C-F30E-4A61-853B-E1A60DB1FA9B}"/>
+      <autoFilter ref="A2:F2" xr:uid="{A55EC0FA-BD10-44CA-990C-59A6546F5CF1}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Add upload so (no data validation)
</commit_message>
<xml_diff>
--- a/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
+++ b/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/AICA008_Incoming List (Supplier)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7B2CE3-81D5-4E3A-B4B2-4C985BE20399}"/>
+  <xr:revisionPtr revIDLastSave="224" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C246B9B-46ED-472A-A3B3-DB61711D5189}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>FG-01-4136-1-250-1</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>FG-01-4136-1-BULK-0</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Note for line 18</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -940,7 +940,7 @@
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="12" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -997,7 +997,7 @@
       <c r="A13" s="3">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1023,7 +1023,7 @@
       <c r="A14" s="3">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1049,7 +1049,7 @@
       <c r="A15" s="3">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1071,7 +1071,7 @@
       <c r="A16" s="3">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1093,8 +1093,8 @@
       <c r="A17" s="3">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>47</v>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
@@ -1117,8 +1117,8 @@
       <c r="A18" s="3">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
-        <v>48</v>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -1143,8 +1143,8 @@
       <c r="A19" s="3">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
-        <v>49</v>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
@@ -1165,7 +1165,7 @@
       <c r="A20" s="3">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1191,7 +1191,7 @@
       <c r="A21" s="3">
         <v>9</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1215,7 +1215,7 @@
       <c r="A22" s="3">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1241,136 +1241,160 @@
       <c r="A23" s="3">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="4">
         <v>1200</v>
       </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="4">
         <v>1200</v>
       </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="4">
         <v>1200</v>
       </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>14</v>
       </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="4">
         <v>1200</v>
       </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>15</v>
       </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="4">
         <v>250</v>
       </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>16</v>
       </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="4">
         <v>250</v>
       </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="4">
         <v>250</v>
       </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>18</v>
       </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="4">
         <v>1200</v>
       </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
       <c r="H30" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1408,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{A55EC0FA-BD10-44CA-990C-59A6546F5CF1}"/>
+      <autoFilter ref="A2:F2" xr:uid="{C930D162-0829-419B-A5E2-B6E8E76F91F8}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Success Upload SO and MFG request
</commit_message>
<xml_diff>
--- a/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
+++ b/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
@@ -821,7 +821,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1408,7 +1408,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{C930D162-0829-419B-A5E2-B6E8E76F91F8}"/>
+      <autoFilter ref="A2:F2" xr:uid="{DF2C3712-878D-4534-B13B-B4E7418EF8B4}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">

</xml_diff>

<commit_message>
1. Fix error of QC detail | 2. Add copy feature to item data, supplier | 3. Add display logic to show item name (Sales order, Work order) | 4. Add item selection modal to incoming, Work order
</commit_message>
<xml_diff>
--- a/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
+++ b/NMVS/uploads/ICLS01_Incoming List (Supplier).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/AICA008_Incoming List (Supplier)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C246B9B-46ED-472A-A3B3-DB61711D5189}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A168EB-409F-42BC-A0C6-58B7EA63222A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Item code</t>
   </si>
@@ -127,36 +127,6 @@
     <t>REF20210915</t>
   </si>
   <si>
-    <t>Note for line 1</t>
-  </si>
-  <si>
-    <t>Note for line 2</t>
-  </si>
-  <si>
-    <t>Note for line 3</t>
-  </si>
-  <si>
-    <t>Note for line 4</t>
-  </si>
-  <si>
-    <t>Note for line 5</t>
-  </si>
-  <si>
-    <t>Note for line 6</t>
-  </si>
-  <si>
-    <t>Note for line 7</t>
-  </si>
-  <si>
-    <t>Note for line 8</t>
-  </si>
-  <si>
-    <t>Note for line 9</t>
-  </si>
-  <si>
-    <t>Note for line 10</t>
-  </si>
-  <si>
     <t>L0916</t>
   </si>
   <si>
@@ -217,31 +187,10 @@
     <t>RW-09-8704-2-10-0</t>
   </si>
   <si>
-    <t>Note for line 11</t>
-  </si>
-  <si>
-    <t>Note for line 12</t>
-  </si>
-  <si>
-    <t>Note for line 13</t>
-  </si>
-  <si>
-    <t>Note for line 14</t>
-  </si>
-  <si>
-    <t>Note for line 15</t>
-  </si>
-  <si>
-    <t>Note for line 16</t>
-  </si>
-  <si>
-    <t>Note for line 17</t>
-  </si>
-  <si>
-    <t>Note for line 18</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Luu y hang de vo</t>
   </si>
 </sst>
 </file>
@@ -820,8 +769,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -862,7 +811,7 @@
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -888,7 +837,7 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="8">
-        <v>44454</v>
+        <v>44543</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -927,7 +876,7 @@
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="8">
-        <v>44459</v>
+        <v>44543</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -936,11 +885,11 @@
     </row>
     <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="12" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -998,16 +947,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4">
-        <v>1200</v>
+        <v>10000</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>28</v>
@@ -1016,7 +965,7 @@
         <v>44454</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1024,13 +973,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4">
         <v>1200</v>
@@ -1041,60 +990,54 @@
       <c r="G14" s="10">
         <v>44454</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E15" s="4">
         <v>1200</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4">
         <v>1200</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
@@ -1109,22 +1052,20 @@
       <c r="G17" s="10">
         <v>44454</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E18" s="4">
         <v>1200</v>
@@ -1135,44 +1076,40 @@
       <c r="G18" s="10">
         <v>44454</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E19" s="4">
         <v>1200</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4">
         <v>1200</v>
@@ -1183,16 +1120,14 @@
       <c r="G20" s="10">
         <v>44454</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
@@ -1207,22 +1142,20 @@
       <c r="G21" s="10">
         <v>44454</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E22" s="4">
         <v>250</v>
@@ -1233,19 +1166,17 @@
       <c r="G22" s="10">
         <v>44454</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="4">
@@ -1253,19 +1184,17 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="4">
@@ -1273,16 +1202,14 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>24</v>
@@ -1293,16 +1220,14 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>23</v>
@@ -1313,16 +1238,14 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>22</v>
@@ -1333,16 +1256,14 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>21</v>
@@ -1353,16 +1274,14 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
@@ -1373,16 +1292,14 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>19</v>
@@ -1393,9 +1310,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="H30" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:F22">
@@ -1408,7 +1323,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{DF2C3712-878D-4534-B13B-B4E7418EF8B4}"/>
+      <autoFilter ref="A2:F2" xr:uid="{940EE6C9-22AF-4556-A30B-521276CC57A0}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">

</xml_diff>